<commit_message>
Add: Caso2 - Escenario IFrames
</commit_message>
<xml_diff>
--- a/src/test/resources/datadriven/prueba.xlsx
+++ b/src/test/resources/datadriven/prueba.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AutoProject\prueba-tecnica-web\src\test\resources\datadriven\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86708D21-7935-440B-84E4-5596BC069DE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B316714-0725-4C73-A7E3-94E3D9A0CCD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11295" xr2:uid="{B9F78849-2DB6-4E6B-818F-E8D2F36420E4}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{B9F78849-2DB6-4E6B-818F-E8D2F36420E4}"/>
   </bookViews>
   <sheets>
     <sheet name="Scenario1" sheetId="1" r:id="rId1"/>
+    <sheet name="Scenario2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="9">
   <si>
     <t>username</t>
   </si>
@@ -57,6 +58,12 @@
   </si>
   <si>
     <t>Test01</t>
+  </si>
+  <si>
+    <t>MartiQA</t>
+  </si>
+  <si>
+    <t>Pepe1234#</t>
   </si>
 </sst>
 </file>
@@ -430,8 +437,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FF5DD36-1DE4-472D-8236-83A54B3690E9}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -468,4 +475,48 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1949FBF6-1A8A-46F2-BDD1-BBC023A5A9AE}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add: Caso2 Completed and Optimized imports
</commit_message>
<xml_diff>
--- a/src/test/resources/datadriven/prueba.xlsx
+++ b/src/test/resources/datadriven/prueba.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AutoProject\prueba-tecnica-web\src\test\resources\datadriven\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B316714-0725-4C73-A7E3-94E3D9A0CCD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E467FB9D-8E79-4B06-BB6A-717337CC183D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{B9F78849-2DB6-4E6B-818F-E8D2F36420E4}"/>
+    <workbookView xWindow="720" yWindow="4185" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{B9F78849-2DB6-4E6B-818F-E8D2F36420E4}"/>
   </bookViews>
   <sheets>
     <sheet name="Scenario1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="29">
   <si>
     <t>username</t>
   </si>
@@ -60,10 +60,70 @@
     <t>Test01</t>
   </si>
   <si>
-    <t>MartiQA</t>
-  </si>
-  <si>
-    <t>Pepe1234#</t>
+    <t>email</t>
+  </si>
+  <si>
+    <t>gender</t>
+  </si>
+  <si>
+    <t>mobile</t>
+  </si>
+  <si>
+    <t>date-of-birth</t>
+  </si>
+  <si>
+    <t>subject</t>
+  </si>
+  <si>
+    <t>hobbies</t>
+  </si>
+  <si>
+    <t>current-address</t>
+  </si>
+  <si>
+    <t>state</t>
+  </si>
+  <si>
+    <t>city</t>
+  </si>
+  <si>
+    <t>prueba@yopmail.com</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>Aspirante</t>
+  </si>
+  <si>
+    <t>Music</t>
+  </si>
+  <si>
+    <t>Autopista Norte al oriente</t>
+  </si>
+  <si>
+    <t>Haryana</t>
+  </si>
+  <si>
+    <t>karnal</t>
+  </si>
+  <si>
+    <t>Prueba01</t>
+  </si>
+  <si>
+    <t>firstnamePF</t>
+  </si>
+  <si>
+    <t>lastnamePF</t>
+  </si>
+  <si>
+    <t>20/09/2000</t>
+  </si>
+  <si>
+    <t>Test02</t>
+  </si>
+  <si>
+    <t>test02</t>
   </si>
 </sst>
 </file>
@@ -99,8 +159,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -479,7 +540,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1949FBF6-1A8A-46F2-BDD1-BBC023A5A9AE}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
@@ -487,7 +548,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -500,19 +561,85 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1" t="s">
+        <v>13</v>
+      </c>
+      <c r="L1" t="s">
+        <v>14</v>
+      </c>
+      <c r="M1" t="s">
+        <v>15</v>
+      </c>
+      <c r="N1" t="s">
+        <v>24</v>
+      </c>
+      <c r="O1" t="s">
+        <v>25</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>28</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="D2" t="s">
-        <v>6</v>
+        <v>27</v>
+      </c>
+      <c r="E2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2">
+        <v>3004441234</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K2" t="s">
+        <v>20</v>
+      </c>
+      <c r="L2" t="s">
+        <v>21</v>
+      </c>
+      <c r="M2" t="s">
+        <v>22</v>
+      </c>
+      <c r="N2" t="s">
+        <v>23</v>
+      </c>
+      <c r="O2" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>